<commit_message>
Se incorpora icono, validador de campo en blanco, mejora de ruta
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Equipo" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -373,19 +373,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ejemplo</t>
+          <t>Eddie</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>Espinoza</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>